<commit_message>
Dense Trajectory with HOG+Fisher Vector
Get the art-of-state performance!
</commit_message>
<xml_diff>
--- a/KTHActionRecognition/test.xlsx
+++ b/KTHActionRecognition/test.xlsx
@@ -326,13 +326,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -362,6 +362,1686 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> over KTH Database</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25555555555555554"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hu-Moment Vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hu-Moment with Bag of Words</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.87250000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SIFT with Bag of Words</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SIFT with Bag of Words and Spatial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HOG with Bag of Words and Spatial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dense Trajectory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>boxing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>handclapping</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jogging</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>running</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>walking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1768580080"/>
+        <c:axId val="1768580624"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="1">
+                        <c:v>boxing</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>handclapping</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>jogging</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>running</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>walking</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$2:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="1">
+                        <c:v>boxing</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>handclapping</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>jogging</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>running</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>walking</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$2:$F$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="1">
+                        <c:v>boxing</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>handclapping</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>jogging</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>running</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>walking</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$H$2:$H$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$J$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="1">
+                        <c:v>boxing</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>handclapping</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>jogging</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>running</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>walking</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$J$2:$J$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="10"/>
+                <c:order val="10"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="1">
+                        <c:v>boxing</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>handclapping</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>jogging</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>running</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>walking</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$L$2:$L$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1768580080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768580624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1768580624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768580080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -696,15 +2376,15 @@
       <c r="E3" s="13">
         <v>1</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="13">
         <v>1</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="13">
         <v>1</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="12">
         <v>0.92</v>
       </c>
@@ -728,7 +2408,7 @@
       <c r="G4" s="13">
         <v>0.96</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="12">
         <v>0.8</v>
       </c>
@@ -752,7 +2432,7 @@
       <c r="E5" s="13">
         <v>0.84</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="12">
         <v>0.72</v>
       </c>
@@ -784,7 +2464,7 @@
       <c r="G6" s="13">
         <v>1</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="12">
         <v>0.96</v>
       </c>
@@ -805,22 +2485,22 @@
         <v>0.96</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" s="15">
+      <c r="E7" s="16">
         <v>0.88</v>
       </c>
       <c r="F7" s="18"/>
-      <c r="G7" s="15">
+      <c r="G7" s="16">
         <v>0.92</v>
       </c>
       <c r="H7" s="18"/>
-      <c r="I7" s="15">
+      <c r="I7" s="16">
         <v>0.76</v>
       </c>
       <c r="J7" s="18"/>
-      <c r="K7" s="15">
+      <c r="K7" s="16">
         <v>0.92</v>
       </c>
-      <c r="L7" s="16"/>
+      <c r="L7" s="17"/>
     </row>
     <row r="8" spans="1:12" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
@@ -861,5 +2541,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>